<commit_message>
Evaluated SMT BOM List for JLPCB
</commit_message>
<xml_diff>
--- a/DSP_MainBoard/JLPCB_Odered/FreeDSP_Catamaran_BOM1.xlsx
+++ b/DSP_MainBoard/JLPCB_Odered/FreeDSP_Catamaran_BOM1.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HILO/Documents/KICAD_DATA/ADAU1701/FreeDSP_Catamaran/DSP_MainBoard/Source/JLPCB_Odered/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AA87A8-0BB3-A84A-AE19-3D0813CC7369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96ACA85-0E4D-BB4B-8F8B-47EDB3CAA6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="4240" windowWidth="34980" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12820" yWindow="6400" windowWidth="34980" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SMD" sheetId="2" r:id="rId1"/>
+    <sheet name="SMD for 0v22" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SMD!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SMD for 0v22'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="307">
   <si>
     <t xml:space="preserve">    C21</t>
   </si>
@@ -392,9 +392,6 @@
   </si>
   <si>
     <t xml:space="preserve">    IC2</t>
-  </si>
-  <si>
-    <t>24AA256</t>
   </si>
   <si>
     <t>Housings_SOIC:SOIC-8_3.9x4.9mm_Pitch1.27mm</t>
@@ -973,12 +970,38 @@
   <si>
     <t>S3D12.288000B20F30T</t>
   </si>
+  <si>
+    <t>OPA1652</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C30025</t>
+  </si>
+  <si>
+    <t>18k</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C17506</t>
+  </si>
+  <si>
+    <t>1k</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>24AA256(or CAT24M01WI-GT3)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C152172</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1021,6 +1044,14 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1059,7 +1090,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1079,6 +1110,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1398,8 +1435,8 @@
   <dimension ref="A1:D201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A202" sqref="A202"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1412,16 +1449,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21">
@@ -1454,16 +1491,16 @@
     </row>
     <row r="4" spans="1:4" ht="21">
       <c r="A4" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="21">
@@ -1538,16 +1575,16 @@
     </row>
     <row r="10" spans="1:4" ht="21">
       <c r="A10" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="21">
@@ -1566,16 +1603,16 @@
     </row>
     <row r="12" spans="1:4" ht="21">
       <c r="A12" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="21">
@@ -1622,16 +1659,16 @@
     </row>
     <row r="16" spans="1:4" ht="21">
       <c r="A16" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="21">
@@ -1748,16 +1785,16 @@
     </row>
     <row r="25" spans="1:4" ht="21">
       <c r="A25" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="21">
@@ -2056,16 +2093,16 @@
     </row>
     <row r="47" spans="1:4" ht="21">
       <c r="A47" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="21">
@@ -2126,16 +2163,16 @@
     </row>
     <row r="52" spans="1:4" ht="21">
       <c r="A52" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="21">
@@ -2224,16 +2261,16 @@
     </row>
     <row r="59" spans="1:4" ht="21">
       <c r="A59" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="21">
@@ -2247,7 +2284,7 @@
         <v>95</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="21">
@@ -2261,329 +2298,329 @@
         <v>95</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="21">
       <c r="A62" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="21">
       <c r="A63" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="21">
       <c r="A64" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="21">
       <c r="A65" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="21">
       <c r="A66" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="21">
       <c r="A67" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C67" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="21">
       <c r="A68" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C68" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="21">
       <c r="A69" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="21">
       <c r="A70" s="5" t="s">
-        <v>119</v>
+        <v>305</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>118</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>121</v>
+        <v>306</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="21">
       <c r="A71" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C71" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="21">
       <c r="A72" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C72" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="21">
       <c r="A73" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="D73" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="21">
       <c r="A74" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="21">
       <c r="A75" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D75" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="21">
       <c r="A76" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D76" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="21">
       <c r="A77" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="21">
       <c r="A78" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="21">
       <c r="A79" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="D79" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="21">
       <c r="A80" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="D80" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="21">
       <c r="A81" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D81" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="21">
       <c r="A82" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="D82" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="21">
       <c r="A83" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C83" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="21">
       <c r="A84" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="21">
@@ -2602,16 +2639,16 @@
     </row>
     <row r="86" spans="1:4" ht="21">
       <c r="A86" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="21">
@@ -2619,7 +2656,7 @@
         <v>38</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>27</v>
@@ -2633,7 +2670,7 @@
         <v>38</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>27</v>
@@ -2647,7 +2684,7 @@
         <v>38</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>27</v>
@@ -2661,7 +2698,7 @@
         <v>38</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>27</v>
@@ -2675,7 +2712,7 @@
         <v>38</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>27</v>
@@ -2689,7 +2726,7 @@
         <v>38</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>27</v>
@@ -2703,7 +2740,7 @@
         <v>38</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>27</v>
@@ -2714,44 +2751,44 @@
     </row>
     <row r="94" spans="1:4" ht="21">
       <c r="A94" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D94" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="21">
       <c r="A95" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D95" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="21">
       <c r="A96" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D96" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="21">
@@ -2770,16 +2807,16 @@
     </row>
     <row r="98" spans="1:4" ht="21">
       <c r="A98" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D98" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="21">
@@ -2938,16 +2975,16 @@
     </row>
     <row r="110" spans="1:4" ht="21">
       <c r="A110" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D110" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="21">
@@ -2980,16 +3017,16 @@
     </row>
     <row r="113" spans="1:4" ht="21">
       <c r="A113" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D113" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="21">
@@ -3119,8 +3156,8 @@
       </c>
     </row>
     <row r="123" spans="1:4" ht="21">
-      <c r="A123" s="5" t="s">
-        <v>38</v>
+      <c r="A123" s="7" t="s">
+        <v>302</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>47</v>
@@ -3128,27 +3165,27 @@
       <c r="C123" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D123" s="2" t="s">
-        <v>39</v>
+      <c r="D123" s="8" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="21">
       <c r="A124" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D124" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B124" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>161</v>
-      </c>
     </row>
     <row r="125" spans="1:4" ht="21">
-      <c r="A125" s="5" t="s">
-        <v>38</v>
+      <c r="A125" s="7" t="s">
+        <v>302</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>48</v>
@@ -3156,22 +3193,22 @@
       <c r="C125" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D125" s="2" t="s">
-        <v>39</v>
+      <c r="D125" s="8" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="21">
       <c r="A126" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D126" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="21">
@@ -3232,16 +3269,16 @@
     </row>
     <row r="131" spans="1:4" ht="21">
       <c r="A131" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D131" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="21">
@@ -3274,16 +3311,16 @@
     </row>
     <row r="134" spans="1:4" ht="21">
       <c r="A134" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D134" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="21">
@@ -3301,8 +3338,8 @@
       </c>
     </row>
     <row r="136" spans="1:4" ht="21">
-      <c r="A136" s="5" t="s">
-        <v>38</v>
+      <c r="A136" s="7" t="s">
+        <v>302</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>51</v>
@@ -3310,8 +3347,8 @@
       <c r="C136" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D136" s="2" t="s">
-        <v>39</v>
+      <c r="D136" s="8" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="21">
@@ -3344,30 +3381,30 @@
     </row>
     <row r="139" spans="1:4" ht="21">
       <c r="A139" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="21">
       <c r="A140" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D140" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="21">
@@ -3414,30 +3451,30 @@
     </row>
     <row r="144" spans="1:4" ht="21">
       <c r="A144" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D144" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D144" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="21">
       <c r="A145" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D145" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C145" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D145" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="21">
@@ -3445,7 +3482,7 @@
         <v>38</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>27</v>
@@ -3456,16 +3493,16 @@
     </row>
     <row r="147" spans="1:4" ht="21">
       <c r="A147" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D147" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="21">
@@ -3473,7 +3510,7 @@
         <v>38</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>27</v>
@@ -3487,7 +3524,7 @@
         <v>84</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>27</v>
@@ -3515,7 +3552,7 @@
         <v>84</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>27</v>
@@ -3529,7 +3566,7 @@
         <v>38</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>27</v>
@@ -3540,16 +3577,16 @@
     </row>
     <row r="153" spans="1:4" ht="21">
       <c r="A153" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D153" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="B153" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D153" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="21">
@@ -3557,7 +3594,7 @@
         <v>107</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>27</v>
@@ -3571,7 +3608,7 @@
         <v>107</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C155" s="2" t="s">
         <v>27</v>
@@ -3582,44 +3619,44 @@
     </row>
     <row r="156" spans="1:4" ht="21">
       <c r="A156" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D156" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D156" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="21">
       <c r="A157" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="21">
       <c r="A158" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="21">
@@ -3641,7 +3678,7 @@
         <v>84</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>27</v>
@@ -3652,16 +3689,16 @@
     </row>
     <row r="161" spans="1:4" ht="21">
       <c r="A161" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D161" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D161" s="2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="21">
@@ -3669,7 +3706,7 @@
         <v>38</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>27</v>
@@ -3680,30 +3717,30 @@
     </row>
     <row r="163" spans="1:4" ht="21">
       <c r="A163" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C163" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="21">
       <c r="A164" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D164" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C164" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D164" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="21">
@@ -3711,7 +3748,7 @@
         <v>84</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>27</v>
@@ -3722,30 +3759,30 @@
     </row>
     <row r="166" spans="1:4" ht="21">
       <c r="A166" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D166" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C166" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D166" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="21">
       <c r="A167" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D167" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C167" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D167" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="21">
@@ -3753,7 +3790,7 @@
         <v>84</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>27</v>
@@ -3767,7 +3804,7 @@
         <v>84</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>27</v>
@@ -3792,16 +3829,16 @@
     </row>
     <row r="171" spans="1:4" ht="21">
       <c r="A171" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D171" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D171" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="21">
@@ -3809,7 +3846,7 @@
         <v>26</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>27</v>
@@ -3823,7 +3860,7 @@
         <v>84</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>27</v>
@@ -3837,7 +3874,7 @@
         <v>38</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C174" s="2" t="s">
         <v>27</v>
@@ -3851,7 +3888,7 @@
         <v>26</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>27</v>
@@ -3865,7 +3902,7 @@
         <v>26</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>27</v>
@@ -3879,7 +3916,7 @@
         <v>26</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>27</v>
@@ -3889,45 +3926,45 @@
       </c>
     </row>
     <row r="178" spans="1:4" ht="21">
-      <c r="A178" s="5" t="s">
-        <v>143</v>
+      <c r="A178" s="7" t="s">
+        <v>304</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C178" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D178" s="2" t="s">
-        <v>294</v>
+      <c r="D178" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="21">
       <c r="A179" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B179" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" ht="21">
+      <c r="A180" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="B180" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C179" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D179" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" ht="21">
-      <c r="A180" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="C180" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D180" s="2" t="s">
-        <v>294</v>
+      <c r="D180" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="21">
@@ -3949,7 +3986,7 @@
         <v>38</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>27</v>
@@ -3959,31 +3996,31 @@
       </c>
     </row>
     <row r="183" spans="1:4" ht="21">
-      <c r="A183" s="5" t="s">
-        <v>143</v>
+      <c r="A183" s="7" t="s">
+        <v>304</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C183" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D183" s="2" t="s">
-        <v>294</v>
+      <c r="D183" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="21">
       <c r="A184" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D184" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="C184" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D184" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="21">
@@ -3991,7 +4028,7 @@
         <v>26</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>27</v>
@@ -4002,16 +4039,16 @@
     </row>
     <row r="186" spans="1:4" ht="21">
       <c r="A186" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="21">
@@ -4019,7 +4056,7 @@
         <v>107</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>27</v>
@@ -4033,7 +4070,7 @@
         <v>107</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>27</v>
@@ -4047,7 +4084,7 @@
         <v>107</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>27</v>
@@ -4061,7 +4098,7 @@
         <v>107</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C190" s="2" t="s">
         <v>27</v>
@@ -4075,7 +4112,7 @@
         <v>38</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C191" s="2" t="s">
         <v>27</v>
@@ -4086,142 +4123,142 @@
     </row>
     <row r="192" spans="1:4" ht="21">
       <c r="A192" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C192" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B192" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="C192" s="2" t="s">
-        <v>221</v>
-      </c>
       <c r="D192" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="21">
       <c r="A193" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C193" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B193" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="C193" s="2" t="s">
+      <c r="D193" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="D193" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="21">
       <c r="A194" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C194" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B194" s="2" t="s">
+      <c r="D194" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" ht="21">
+      <c r="A195" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="B195" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C194" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D194" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" ht="21">
-      <c r="A195" s="5" t="s">
+      <c r="C195" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B195" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="C195" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D195" s="2" t="s">
-        <v>298</v>
+      <c r="D195" s="8" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="21">
       <c r="A196" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C196" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B196" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="C196" s="2" t="s">
-        <v>221</v>
-      </c>
       <c r="D196" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="21">
       <c r="A197" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="21">
       <c r="A198" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="21">
       <c r="A199" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C199" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B199" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="C199" s="2" t="s">
-        <v>221</v>
-      </c>
       <c r="D199" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="21">
       <c r="A200" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D200" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B200" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C200" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D200" s="2" t="s">
+    </row>
+    <row r="201" spans="1:4" ht="21">
+      <c r="A201" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B201" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="201" spans="1:4">
-      <c r="A201" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="B201" s="2" t="s">
+      <c r="C201" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C201" s="2" t="s">
-        <v>227</v>
-      </c>
       <c r="D201" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>